<commit_message>
update download employee File
</commit_message>
<xml_diff>
--- a/src/Api/Content/AddEmployees.xlsx
+++ b/src/Api/Content/AddEmployees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Prog-Projects\IProgram\src\Api\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA789B97-2A83-4415-8864-853C3B67D943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED1552B-5BE2-4202-BC25-A74CB71BE2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <t>الكود</t>
   </si>
   <si>
-    <t>اسم القسم</t>
+    <t>أسم القسم</t>
   </si>
 </sst>
 </file>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F308BE0-E2B9-4AA3-B943-124106509D1D}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>